<commit_message>
Tested algorithms & revamped quickSort algorithm
</commit_message>
<xml_diff>
--- a/lab7/Lab7-Timings.xlsx
+++ b/lab7/Lab7-Timings.xlsx
@@ -1,23 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2030\2030-GA-Files\2030-GA-Files\lab\instructs-NEW\lab7\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Devin_Brewer\OneDrive - University of Wyoming\Classes\Fall 2018\COSC 2030\GitHub (cosc-2030)\lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_CA2A816B5D9327194311C33AE5836A0348175821" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{6BF9541B-9738-4171-9FE6-3B878092B350}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9345" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="179021" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -74,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -413,11 +419,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -479,80 +485,131 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>40000000</v>
       </c>
       <c r="C5">
         <f>2*B5</f>
-        <v>0</v>
+        <v>80000000</v>
+      </c>
+      <c r="D5">
+        <v>8.1</v>
       </c>
       <c r="E5">
         <f>2*C5</f>
-        <v>0</v>
+        <v>160000000</v>
+      </c>
+      <c r="F5">
+        <v>16.21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
+      <c r="B6">
+        <v>1000000</v>
+      </c>
       <c r="C6">
         <f t="shared" ref="C6:C10" si="0">2*B6</f>
-        <v>0</v>
+        <v>2000000</v>
+      </c>
+      <c r="D6">
+        <v>15.67</v>
       </c>
       <c r="E6">
         <f t="shared" ref="E6:E10" si="1">2*C6</f>
-        <v>0</v>
+        <v>4000000</v>
+      </c>
+      <c r="F6">
+        <v>62.45</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
+      <c r="B7">
+        <v>10100</v>
+      </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20200</v>
+      </c>
+      <c r="D7">
+        <v>15.96</v>
       </c>
       <c r="E7">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>40400</v>
+      </c>
+      <c r="F7">
+        <v>63.630899999999997</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>12000</v>
+      </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>24000</v>
+      </c>
+      <c r="D8">
+        <v>16.309999999999999</v>
       </c>
       <c r="E8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>48000</v>
+      </c>
+      <c r="F8">
+        <v>65.42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
+      <c r="B9">
+        <v>13000</v>
+      </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>26000</v>
+      </c>
+      <c r="D9">
+        <v>16.71</v>
       </c>
       <c r="E9">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>52000</v>
+      </c>
+      <c r="F9">
+        <v>66.55</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
+      <c r="B10">
+        <v>250000</v>
+      </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500000</v>
+      </c>
+      <c r="D10">
+        <v>13.12</v>
       </c>
       <c r="E10">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000000</v>
+      </c>
+      <c r="F10">
+        <v>47.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>